<commit_message>
Day 2 Sprint Backlog
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthcarnegie\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A72EF81-33D7-4973-903F-7430E7B1993A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Task Name</t>
   </si>
@@ -174,12 +183,15 @@
   </si>
   <si>
     <t>Marius Urbelis</t>
+  </si>
+  <si>
+    <t>Create scripts to transform simple maps data into SQL script</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,8 +263,8 @@
   <colors>
     <mruColors>
       <color rgb="FF00FFFF"/>
+      <color rgb="FF00FF00"/>
       <color rgb="FF00CCFF"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -528,11 +540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,13 +607,19 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3">
         <v>43864</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>40</v>
+      <c r="G2" s="3">
+        <v>43865</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -635,137 +653,172 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43864</v>
+      </c>
+      <c r="G4" s="3">
+        <v>43864</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43864</v>
+      </c>
+      <c r="G5" s="3">
+        <v>43864</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43864</v>
+      </c>
+      <c r="G6" s="3">
+        <v>43864</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>7</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>41</v>
+      <c r="F7" s="3">
+        <v>43864</v>
+      </c>
+      <c r="G7" s="3">
+        <v>43865</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43864</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>43865</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>43865</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>40</v>
@@ -773,19 +826,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>41</v>
@@ -793,19 +846,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>41</v>
@@ -813,19 +866,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>41</v>
@@ -833,19 +886,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>41</v>
@@ -853,16 +906,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -873,34 +926,54 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
       </c>
       <c r="E17">
-        <f>SUM(E2:E16)</f>
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>SUM(E2:E17)</f>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J18">
+    <sortCondition ref="I6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>